<commit_message>
Reading the excel file
</commit_message>
<xml_diff>
--- a/nutri.xlsx
+++ b/nutri.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vidit\Documents\p8105_final_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{94EA69E1-AE53-438C-A663-10390A53EC05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{453C1CE3-F7C3-48CC-AC5D-20E5B3DEFC32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{3662D4D2-8B5D-4455-B495-B61141140925}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="74">
   <si>
     <t>Downloaded from</t>
   </si>
@@ -229,9 +229,6 @@
     <t>Fat free</t>
   </si>
   <si>
-    <t>WHOLE</t>
-  </si>
-  <si>
     <t>Skim</t>
   </si>
   <si>
@@ -266,6 +263,12 @@
   </si>
   <si>
     <t>Vitamin C [Ascorbic acid] (mg)</t>
+  </si>
+  <si>
+    <t>2 Percent</t>
+  </si>
+  <si>
+    <t>1 Percent</t>
   </si>
 </sst>
 </file>
@@ -624,7 +627,7 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -638,16 +641,16 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E1" t="s">
         <v>60</v>
-      </c>
-      <c r="C1" s="2">
-        <v>0.02</v>
-      </c>
-      <c r="D1" s="2">
-        <v>0.01</v>
-      </c>
-      <c r="E1" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -669,7 +672,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B3">
         <v>1.2</v>
@@ -686,7 +689,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B4">
         <v>300</v>
@@ -703,7 +706,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -720,7 +723,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B6">
         <v>124.8</v>
@@ -737,7 +740,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B7">
         <v>7.99</v>
@@ -754,7 +757,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B8">
         <v>13.01</v>
@@ -771,7 +774,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -788,7 +791,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B10">
         <v>12</v>
@@ -805,7 +808,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B11">
         <v>13.01</v>
@@ -822,7 +825,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B12">
         <v>36</v>
@@ -839,7 +842,7 @@
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Nutrition related plotting first attempt/ analysis
</commit_message>
<xml_diff>
--- a/nutri.xlsx
+++ b/nutri.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vidit\Documents\p8105_final_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{453C1CE3-F7C3-48CC-AC5D-20E5B3DEFC32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B4008F7-59F9-4853-AEBE-FF4D7474F161}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{3662D4D2-8B5D-4455-B495-B61141140925}"/>
+    <workbookView xWindow="3516" yWindow="3516" windowWidth="17280" windowHeight="9960" xr2:uid="{3662D4D2-8B5D-4455-B495-B61141140925}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="75">
   <si>
     <t>Downloaded from</t>
   </si>
@@ -269,6 +269,9 @@
   </si>
   <si>
     <t>1 Percent</t>
+  </si>
+  <si>
+    <t>Nutritional Components</t>
   </si>
 </sst>
 </file>
@@ -626,9 +629,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0887506D-354C-4228-9F12-DE60E131A157}">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -640,6 +641,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>74</v>
+      </c>
       <c r="B1" t="s">
         <v>52</v>
       </c>

</xml_diff>